<commit_message>
LinkedIn API Final Version
</commit_message>
<xml_diff>
--- a/sales_navigator/LinkedIn_Data/LinkedIn_Sales_Navigator_Data_Limit10.xlsx
+++ b/sales_navigator/LinkedIn_Data/LinkedIn_Sales_Navigator_Data_Limit10.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hussain\Projects\Scraping Work\Dmitri Work\sales_navigator\LinkedIn_Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70996AAE-9FFE-4A2F-B7B2-6FD0CB8FB798}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -178,8 +184,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +261,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -301,7 +315,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,9 +347,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,6 +399,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -542,239 +592,217 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
         <v>26</v>
       </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
       <c r="F2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="G2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1">
-        <v>9</v>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
         <v>35</v>
       </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
       <c r="F11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>